<commit_message>
added info, notes, appendix
</commit_message>
<xml_diff>
--- a/docs/timeline-effortmatrix.xlsx
+++ b/docs/timeline-effortmatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\School\Fall 22'\Senior Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\School\Fall 22'\Senior Design\Repo\uc-senior-design\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8A1DA5-7510-4ECA-A020-8AAD29CA5DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA4DEEB-AFB1-4ED6-85BA-70A7A0E929D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17620" xr2:uid="{0F6331A5-7373-468F-9337-F150DB4F1D31}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="38700" windowHeight="15285" xr2:uid="{0F6331A5-7373-468F-9337-F150DB4F1D31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
     <t>Nov 15 - Dec 15</t>
   </si>
   <si>
-    <t>1 - 15</t>
-  </si>
-  <si>
     <t>Jan 15 - Feb 15</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>Effort by Nick A</t>
+  </si>
+  <si>
+    <t>9-15</t>
   </si>
 </sst>
 </file>
@@ -181,20 +181,8 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -202,6 +190,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,33 +519,33 @@
   <dimension ref="B1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="D1" s="1">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D1" s="6">
         <v>2022</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6">
         <v>2023</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -572,147 +572,147 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9">
-        <v>1</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="9">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="9">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="9">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="9">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="9">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="9">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="9">
-        <v>1</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="9">
-        <v>1</v>
-      </c>
-      <c r="J15" s="8"/>
-      <c r="K15" s="2">
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>